<commit_message>
Arquivo excel sendo lido e valores já sendo colocados nos devidos locais. Iniciado próxima feat.
</commit_message>
<xml_diff>
--- a/clockify/clockify_database.xlsx
+++ b/clockify/clockify_database.xlsx
@@ -50,7 +50,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -83,17 +83,17 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="167" formatCode="h:mm;@"/>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="h:mm;@"/>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -410,7 +410,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adicionado a função get_login_clockify para melhor compreensão do código da função do_login_clockify. Adicionado verificação de login com a imagem clockify_work_page
</commit_message>
<xml_diff>
--- a/clockify/clockify_database.xlsx
+++ b/clockify/clockify_database.xlsx
@@ -90,9 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +420,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,8 +454,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2104</v>
+      <c r="A2" s="2">
+        <v>45037</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -473,8 +474,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2104</v>
+      <c r="A3" s="2">
+        <v>45037</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -493,8 +494,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2104</v>
+      <c r="A4" s="2">
+        <v>45038</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -513,8 +514,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2104</v>
+      <c r="A5" s="2">
+        <v>45039</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>

</xml_diff>